<commit_message>
vehicle import brnad import + some minor fixes, added cartype tabel
</commit_message>
<xml_diff>
--- a/public/Vehicle Sample.xlsx
+++ b/public/Vehicle Sample.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">sedan</t>
   </si>
   <si>
-    <t xml:space="preserve">Hundai</t>
+    <t xml:space="preserve">Hyundai</t>
   </si>
   <si>
     <t xml:space="preserve">sonata</t>
@@ -112,9 +112,6 @@
     <t xml:space="preserve">18729D</t>
   </si>
   <si>
-    <t xml:space="preserve">hundai</t>
-  </si>
-  <si>
     <t xml:space="preserve">accent</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
     <t xml:space="preserve">11119D</t>
   </si>
   <si>
+    <t xml:space="preserve">hyundai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Creta</t>
   </si>
   <si>
@@ -172,10 +172,10 @@
     <t xml:space="preserve">90818729D</t>
   </si>
   <si>
+    <t xml:space="preserve">4WD</t>
+  </si>
+  <si>
     <t xml:space="preserve">jeep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wrangler</t>
   </si>
   <si>
     <t xml:space="preserve">76718729D</t>
@@ -261,12 +261,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,13 +291,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -535,10 +539,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2006</v>
@@ -574,18 +578,18 @@
         <v>20</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2016</v>
@@ -621,15 +625,15 @@
         <v>20</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -675,8 +679,8 @@
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -769,8 +773,8 @@
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>44</v>
@@ -816,8 +820,8 @@
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -911,7 +915,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>51</v>
@@ -953,6 +957,7 @@
         <v>52</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>